<commit_message>
cambio test run MotorSinUBER
</commit_message>
<xml_diff>
--- a/SuraClaims/Validacion_GeneracionSiniestro_SISE.xlsx
+++ b/SuraClaims/Validacion_GeneracionSiniestro_SISE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74F5AD7-B2A9-4C7F-986C-8AC742CD5031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ABA67C-2C65-481A-B990-B6CD77DF88D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{77A7D9F1-F7BA-4199-BEE8-4F39B1D5E954}"/>
   </bookViews>
@@ -60,16 +60,16 @@
     <t>0420172010228</t>
   </si>
   <si>
-    <t xml:space="preserve">0420194406895   </t>
-  </si>
-  <si>
-    <t>0420194406896</t>
-  </si>
-  <si>
-    <t>1120170200973</t>
-  </si>
-  <si>
-    <t>1220194200691</t>
+    <t xml:space="preserve">0420194407302   </t>
+  </si>
+  <si>
+    <t>0420194407303</t>
+  </si>
+  <si>
+    <t>1220194200722</t>
+  </si>
+  <si>
+    <t>1120194100457</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>